<commit_message>
Final commit with v1
</commit_message>
<xml_diff>
--- a/result.xlsx
+++ b/result.xlsx
@@ -345,7 +345,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -375,6 +375,28 @@
         </is>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>1998D000001</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Rojas Nancy</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Cochran Oscar</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>1998-02-01</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Added the case activity part
</commit_message>
<xml_diff>
--- a/result.xlsx
+++ b/result.xlsx
@@ -345,7 +345,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -397,6 +397,138 @@
         </is>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>1998D000002</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Jubiter Gloria</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Jubiter Michael, Mcgee Michael</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>1998-02-01</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>1998D000003</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Berryhill Cloris</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Berryhill Kenneth E</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>1998-02-01</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>1998D000005</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Leeper Stacey</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Leeper Glenn</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>1998-02-01</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>1998D000006</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Allen Aubrey</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Ross Barbara</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>1998-02-01</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>1998D000007</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Cartier Diana</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Delon Michael</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>1998-02-01</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>1998D000008</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Koons Sandra</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Koons Sam</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>1998-02-01</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Changed some files, and added the utils folder to contain the utils
</commit_message>
<xml_diff>
--- a/result.xlsx
+++ b/result.xlsx
@@ -345,7 +345,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:D38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -400,17 +400,17 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>1998D000002</t>
+          <t>1998D000010</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Jubiter Gloria</t>
+          <t>Jarecki Yvonne</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Jubiter Michael, Mcgee Michael</t>
+          <t>Jarecki Lawrence</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -422,17 +422,17 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>1998D000003</t>
+          <t>1998D000016</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Berryhill Cloris</t>
+          <t>Boutros Shamshoun</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Berryhill Kenneth E</t>
+          <t>Boutros Helen</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -444,17 +444,17 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>1998D000005</t>
+          <t>1998D000018</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Leeper Stacey</t>
+          <t>Galloway Corey</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Leeper Glenn</t>
+          <t>Pitts Tamika</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -466,17 +466,17 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>1998D000006</t>
+          <t>1998D000002</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Allen Aubrey</t>
+          <t>Jubiter Gloria</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Ross Barbara</t>
+          <t>Jubiter Michael, Mcgee Michael</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -488,17 +488,17 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>1998D000007</t>
+          <t>1998D000020</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Cartier Diana</t>
+          <t>Woehlke Nancy J</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Delon Michael</t>
+          <t>Woehlke Charles M</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -510,20 +510,680 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
+          <t>1998D000021</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Rowe Beverly</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Rowe Julian</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>1998-02-01</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>1998D000022</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Lee Steven</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Sangerman Zoe</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>1998-02-01</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>1998D000023</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Minnifield Barbara</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Minnifield Terry</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>1998-02-01</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>1998D000026</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Kushner Mark</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>Kushner Ellen</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>1998-02-01</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>1998D000028</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Pedersen John</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>Pedersen Flora</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>1998-02-01</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>1998D000029</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Tsusaki Pamela</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>Tsusaki Dean</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>1998-02-01</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>1998D000003</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Berryhill Cloris</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>Berryhill Kenneth E</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>1998-02-01</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>1998D000030</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Pacheco Anthony</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>Pacheco Christina</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>1998-02-01</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>1998D000031</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Delahanty Daniel</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>Delahanty Patricia</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>1998-02-01</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>1998D000033</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Lozano Al</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>Lozano Diane</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>1998-02-01</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>1998D000034</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Heard Leslie R</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>Heard Arthur L</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>1998-02-01</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>1998D000035</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>Szymczak Donna</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>Szymczak Daniel</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>1998-02-01</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>1998D000036</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>Miller Betty</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>Mitchell Nick</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>1998-02-01</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>1998D000037</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>Chassagne Jeanpierre</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>Middleton Marybeth</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>1998-02-01</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>1998D000038</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>Mccombs Marianna</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>Mccombs Earl</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>1998-02-01</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>1998D000039</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>Muja Janus</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>Muja Serveta</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>1998-02-01</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>1998D000040</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>Edwards Pamela</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>Allen Gordon</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>1998-02-01</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>1998D000041</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>Winters Denise</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>Winters Clyde</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>1998-02-01</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>1998D000042</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>Stanziola Marielyz</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>Ayersman Jeff</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>1998-02-01</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>1998D000043</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>Fossler Stephen</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>Fossler Francine</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>1998-02-01</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>1998D000044</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>Economou Dimitrios</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>Economou Elzbieta</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>1998-02-01</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>1998D000045</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>Mooth Emeko</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>Mooth Gerald</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>1998-02-01</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>1998D000046</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>Fitzgerald Joseph</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>Matjasko Jennifer</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>1998-02-01</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>1998D000047</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>Huff Constance</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>Huff Fritz</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>1998-02-01</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>1998D000048</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>Wallace Jackie</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>Wallace Samuel</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>1998-05-01</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>1998D000049</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>Dennis Katrina M</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>Dennis Ii Charles B</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>1998-05-01</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>1998D000005</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>Leeper Stacey</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>Leeper Glenn</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>1998-02-01</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>1998D000050</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>Robinson Sylvia</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>Robinson Jr Tim</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>1998-05-01</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>1998D000006</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>Allen Aubrey</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>Ross Barbara</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>1998-02-01</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>1998D000007</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>Cartier Diana</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>Delon Michael</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>1998-02-01</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
           <t>1998D000008</t>
         </is>
       </c>
-      <c r="B8" t="inlineStr">
+      <c r="B38" t="inlineStr">
         <is>
           <t>Koons Sandra</t>
         </is>
       </c>
-      <c r="C8" t="inlineStr">
+      <c r="C38" t="inlineStr">
         <is>
           <t>Koons Sam</t>
         </is>
       </c>
-      <c r="D8" t="inlineStr">
+      <c r="D38" t="inlineStr">
         <is>
           <t>1998-02-01</t>
         </is>

</xml_diff>